<commit_message>
Analyze OpenAI Similarity Distance
</commit_message>
<xml_diff>
--- a/artifacts/gpr-4 self-consistency experiment/result_summary.xlsx
+++ b/artifacts/gpr-4 self-consistency experiment/result_summary.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QUAN\Desktop\medical-chatbot\artifacts\gpr-4 self-consistency experiment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8662A4-9F57-44F5-BF9C-D71AE9948FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22785" windowHeight="14655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="62">
   <si>
     <t>No</t>
   </si>
@@ -208,12 +202,27 @@
   </si>
   <si>
     <t>vedolizumab</t>
+  </si>
+  <si>
+    <t>Relevance Scores</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>TBC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -278,13 +287,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -380,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -557,38 +569,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K14" sqref="E9:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.90625" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" customWidth="1"/>
-    <col min="11" max="11" width="12.90625" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,11 +700,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3">
@@ -790,9 +801,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -875,9 +886,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
@@ -897,9 +908,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
@@ -913,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -1008,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="2">
@@ -1099,7 +1110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1194,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="2">
@@ -1282,7 +1293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>3</v>
       </c>
@@ -1374,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="2">
@@ -1462,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -1560,7 +1571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="2">
@@ -1651,7 +1662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1746,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="2">
@@ -1836,18 +1847,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1855,25 +1866,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C98C75-0D27-447D-AE96-0C32957B5721}">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.90625" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1889,26 +1901,32 @@
       <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+      <c r="F1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1922,32 +1940,38 @@
       <c r="E2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="4">
-        <f>COUNTIF(Raw!$D$6:$D$15,Question!F$1)</f>
-        <v>4</v>
-      </c>
-      <c r="G2" s="8">
-        <f>COUNTIF(Raw!$D$6:$D$15,Question!G$1)</f>
+      <c r="F2" s="9">
+        <v>0.33185646000000002</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="4">
+        <f>COUNTIF(Raw!$D$6:$D$15,Question!H$1)</f>
+        <v>4</v>
+      </c>
+      <c r="I2" s="6">
+        <f>COUNTIF(Raw!$D$6:$D$15,Question!I$1)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="8">
-        <f>COUNTIF(Raw!$D$6:$D$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <f>COUNTIF(Raw!$D$6:$D$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J2" s="8">
+      <c r="J2" s="6">
         <f>COUNTIF(Raw!$D$6:$D$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="4">
         <f>COUNTIF(Raw!$D$6:$D$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L2" s="6">
+        <f>COUNTIF(Raw!$D$6:$D$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <f>COUNTIF(Raw!$D$6:$D$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1961,33 +1985,39 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4">
-        <f>COUNTIF(Raw!$E$6:$E$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G3" s="8">
-        <f>COUNTIF(Raw!$E$6:$E$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
+      <c r="F3" s="9">
+        <v>0.34514626999999998</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="4">
         <f>COUNTIF(Raw!$E$6:$E$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
         <f>COUNTIF(Raw!$E$6:$E$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
         <f>COUNTIF(Raw!$E$6:$E$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="4">
         <f>COUNTIF(Raw!$E$6:$E$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <f>COUNTIF(Raw!$E$6:$E$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <f>COUNTIF(Raw!$E$6:$E$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1999,33 +2029,39 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="8">
-        <f>COUNTIF(Raw!$F$6:$F$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <f>COUNTIF(Raw!$F$6:$F$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="F4" s="9">
+        <v>0.2917188</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="6">
         <f>COUNTIF(Raw!$F$6:$F$15,Question!H$1)</f>
-        <v>2</v>
-      </c>
-      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <f>COUNTIF(Raw!$F$6:$F$15,Question!I$1)</f>
-        <v>3</v>
-      </c>
-      <c r="J4" s="8">
+        <v>5</v>
+      </c>
+      <c r="J4" s="5">
         <f>COUNTIF(Raw!$F$6:$F$15,Question!J$1)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
+        <v>2</v>
+      </c>
+      <c r="K4" s="5">
         <f>COUNTIF(Raw!$F$6:$F$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6">
+        <f>COUNTIF(Raw!$F$6:$F$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <f>COUNTIF(Raw!$F$6:$F$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2039,33 +2075,39 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8">
-        <f>COUNTIF(Raw!$G$6:$G$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <f>COUNTIF(Raw!$G$6:$G$15,Question!G$1)</f>
-        <v>4</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="F5" s="9">
+        <v>0.37213882999999998</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="6">
         <f>COUNTIF(Raw!$G$6:$G$15,Question!H$1)</f>
         <v>0</v>
       </c>
       <c r="I5" s="4">
         <f>COUNTIF(Raw!$G$6:$G$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J5" s="8">
+        <v>4</v>
+      </c>
+      <c r="J5" s="6">
         <f>COUNTIF(Raw!$G$6:$G$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <f>COUNTIF(Raw!$G$6:$G$15,Question!K$1)</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="6">
+        <f>COUNTIF(Raw!$G$6:$G$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K5" s="8">
-        <f>COUNTIF(Raw!$G$6:$G$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M5" s="6">
+        <f>COUNTIF(Raw!$G$6:$G$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2075,32 +2117,38 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4">
-        <f>COUNTIF(Raw!$H$6:$H$15,Question!F$1)</f>
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <f>COUNTIF(Raw!$H$6:$H$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="F6" s="9">
+        <v>0.34616291999999999</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="4">
         <f>COUNTIF(Raw!$H$6:$H$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4">
         <f>COUNTIF(Raw!$H$6:$H$15,Question!I$1)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
         <f>COUNTIF(Raw!$H$6:$H$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="6">
         <f>COUNTIF(Raw!$H$6:$H$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L6" s="6">
+        <f>COUNTIF(Raw!$H$6:$H$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <f>COUNTIF(Raw!$H$6:$H$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2114,32 +2162,38 @@
         <v>4</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="4">
-        <f>COUNTIF(Raw!$I$6:$I$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G7" s="8">
-        <f>COUNTIF(Raw!$I$6:$I$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="F7" s="9">
+        <v>0.35585921999999998</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="4">
         <f>COUNTIF(Raw!$I$6:$I$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6">
         <f>COUNTIF(Raw!$I$6:$I$15,Question!I$1)</f>
-        <v>2</v>
-      </c>
-      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
         <f>COUNTIF(Raw!$I$6:$I$15,Question!J$1)</f>
-        <v>3</v>
-      </c>
-      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
         <f>COUNTIF(Raw!$I$6:$I$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5">
+        <f>COUNTIF(Raw!$I$6:$I$15,Question!L$1)</f>
+        <v>3</v>
+      </c>
+      <c r="M7" s="6">
+        <f>COUNTIF(Raw!$I$6:$I$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2151,32 +2205,38 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4">
-        <f>COUNTIF(Raw!$J$6:$J$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G8" s="8">
-        <f>COUNTIF(Raw!$J$6:$J$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="F8" s="9">
+        <v>0.32789382</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="4">
         <f>COUNTIF(Raw!$J$6:$J$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
         <f>COUNTIF(Raw!$J$6:$J$15,Question!I$1)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="6">
         <f>COUNTIF(Raw!$J$6:$J$15,Question!J$1)</f>
-        <v>5</v>
-      </c>
-      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
         <f>COUNTIF(Raw!$J$6:$J$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L8" s="4">
+        <f>COUNTIF(Raw!$J$6:$J$15,Question!L$1)</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="6">
+        <f>COUNTIF(Raw!$J$6:$J$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2188,32 +2248,38 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="8">
-        <f>COUNTIF(Raw!$K$6:$K$15,Question!F$1)</f>
+      <c r="F9" s="9">
+        <v>0.31963393000000001</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="6">
+        <f>COUNTIF(Raw!$K$6:$K$15,Question!H$1)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <f>COUNTIF(Raw!$K$6:$K$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H9" s="4">
-        <f>COUNTIF(Raw!$K$6:$K$15,Question!H$1)</f>
-        <v>4</v>
-      </c>
-      <c r="I9" s="8">
+      <c r="I9" s="4">
         <f>COUNTIF(Raw!$K$6:$K$15,Question!I$1)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
         <f>COUNTIF(Raw!$K$6:$K$15,Question!J$1)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
+        <v>4</v>
+      </c>
+      <c r="K9" s="6">
         <f>COUNTIF(Raw!$K$6:$K$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L9" s="6">
+        <f>COUNTIF(Raw!$K$6:$K$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <f>COUNTIF(Raw!$K$6:$K$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2225,15 +2291,13 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="8">
-        <f>COUNTIF(Raw!$L$6:$L$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <f>COUNTIF(Raw!$L$6:$L$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="F10" s="9">
+        <v>0.33914640000000001</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="6">
         <f>COUNTIF(Raw!$L$6:$L$15,Question!H$1)</f>
         <v>0</v>
       </c>
@@ -2241,16 +2305,24 @@
         <f>COUNTIF(Raw!$L$6:$L$15,Question!I$1)</f>
         <v>5</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="6">
         <f>COUNTIF(Raw!$L$6:$L$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="4">
         <f>COUNTIF(Raw!$L$6:$L$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L10" s="6">
+        <f>COUNTIF(Raw!$L$6:$L$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <f>COUNTIF(Raw!$L$6:$L$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2262,15 +2334,13 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="8">
-        <f>COUNTIF(Raw!$M$6:$M$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <f>COUNTIF(Raw!$M$6:$M$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="F11" s="9">
+        <v>0.33234823000000002</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="6">
         <f>COUNTIF(Raw!$M$6:$M$15,Question!H$1)</f>
         <v>0</v>
       </c>
@@ -2278,16 +2348,24 @@
         <f>COUNTIF(Raw!$M$6:$M$15,Question!I$1)</f>
         <v>5</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="6">
         <f>COUNTIF(Raw!$M$6:$M$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="4">
         <f>COUNTIF(Raw!$M$6:$M$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L11" s="6">
+        <f>COUNTIF(Raw!$M$6:$M$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <f>COUNTIF(Raw!$M$6:$M$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2299,32 +2377,38 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="8">
-        <f>COUNTIF(Raw!$N$6:$N$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <f>COUNTIF(Raw!$N$6:$N$15,Question!G$1)</f>
-        <v>4</v>
-      </c>
-      <c r="H12" s="8">
+      <c r="F12" s="9">
+        <v>0.32879317000000002</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="6">
         <f>COUNTIF(Raw!$N$6:$N$15,Question!H$1)</f>
         <v>0</v>
       </c>
       <c r="I12" s="4">
         <f>COUNTIF(Raw!$N$6:$N$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J12" s="8">
+        <v>4</v>
+      </c>
+      <c r="J12" s="6">
         <f>COUNTIF(Raw!$N$6:$N$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <f>COUNTIF(Raw!$N$6:$N$15,Question!K$1)</f>
+        <v>5</v>
+      </c>
+      <c r="L12" s="6">
+        <f>COUNTIF(Raw!$N$6:$N$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K12" s="8">
-        <f>COUNTIF(Raw!$N$6:$N$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M12" s="6">
+        <f>COUNTIF(Raw!$N$6:$N$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2336,32 +2420,38 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="8">
-        <f>COUNTIF(Raw!$O$6:$O$15,Question!F$1)</f>
+      <c r="F13" s="9">
+        <v>0.26116722999999997</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="6">
+        <f>COUNTIF(Raw!$O$6:$O$15,Question!H$1)</f>
         <v>1</v>
       </c>
-      <c r="G13" s="8">
-        <f>COUNTIF(Raw!$O$6:$O$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="8">
-        <f>COUNTIF(Raw!$O$6:$O$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="I13" s="6">
         <f>COUNTIF(Raw!$O$6:$O$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
         <f>COUNTIF(Raw!$O$6:$O$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <f>COUNTIF(Raw!$O$6:$O$15,Question!K$1)</f>
+        <v>5</v>
+      </c>
+      <c r="L13" s="6">
+        <f>COUNTIF(Raw!$O$6:$O$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K13" s="8">
-        <f>COUNTIF(Raw!$O$6:$O$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M13" s="6">
+        <f>COUNTIF(Raw!$O$6:$O$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2373,15 +2463,13 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="8">
-        <f>COUNTIF(Raw!$P$6:$P$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <f>COUNTIF(Raw!$P$6:$P$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H14" s="8">
+      <c r="F14" s="9">
+        <v>0.28574699999999997</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="6">
         <f>COUNTIF(Raw!$P$6:$P$15,Question!H$1)</f>
         <v>0</v>
       </c>
@@ -2389,16 +2477,24 @@
         <f>COUNTIF(Raw!$P$6:$P$15,Question!I$1)</f>
         <v>5</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="6">
         <f>COUNTIF(Raw!$P$6:$P$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="4">
         <f>COUNTIF(Raw!$P$6:$P$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L14" s="6">
+        <f>COUNTIF(Raw!$P$6:$P$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <f>COUNTIF(Raw!$P$6:$P$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2412,32 +2508,38 @@
         <v>13</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="4">
-        <f>COUNTIF(Raw!$Q$6:$Q$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G15" s="8">
-        <f>COUNTIF(Raw!$Q$6:$Q$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="8">
+      <c r="F15" s="9">
+        <v>0.32387736</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="4">
         <f>COUNTIF(Raw!$Q$6:$Q$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6">
         <f>COUNTIF(Raw!$Q$6:$Q$15,Question!I$1)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="6">
         <f>COUNTIF(Raw!$Q$6:$Q$15,Question!J$1)</f>
-        <v>5</v>
-      </c>
-      <c r="K15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
         <f>COUNTIF(Raw!$Q$6:$Q$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L15" s="4">
+        <f>COUNTIF(Raw!$Q$6:$Q$15,Question!L$1)</f>
+        <v>5</v>
+      </c>
+      <c r="M15" s="6">
+        <f>COUNTIF(Raw!$Q$6:$Q$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2451,32 +2553,38 @@
         <v>13</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="8">
-        <f>COUNTIF(Raw!$R$6:$R$15,Question!F$1)</f>
-        <v>2</v>
-      </c>
-      <c r="G16" s="8">
-        <f>COUNTIF(Raw!$R$6:$R$15,Question!G$1)</f>
-        <v>2</v>
-      </c>
-      <c r="H16" s="8">
+      <c r="F16" s="9">
+        <v>0.31742910000000002</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="6">
         <f>COUNTIF(Raw!$R$6:$R$15,Question!H$1)</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="6">
+        <f>COUNTIF(Raw!$R$6:$R$15,Question!I$1)</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="6">
+        <f>COUNTIF(Raw!$R$6:$R$15,Question!J$1)</f>
         <v>1</v>
       </c>
-      <c r="I16" s="8">
-        <f>COUNTIF(Raw!$R$6:$R$15,Question!I$1)</f>
+      <c r="K16" s="6">
+        <f>COUNTIF(Raw!$R$6:$R$15,Question!K$1)</f>
         <v>1</v>
       </c>
-      <c r="J16" s="8">
-        <f>COUNTIF(Raw!$R$6:$R$15,Question!J$1)</f>
-        <v>2</v>
-      </c>
-      <c r="K16" s="8">
-        <f>COUNTIF(Raw!$R$6:$R$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="6">
+        <f>COUNTIF(Raw!$R$6:$R$15,Question!L$1)</f>
+        <v>2</v>
+      </c>
+      <c r="M16" s="6">
+        <f>COUNTIF(Raw!$R$6:$R$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2490,32 +2598,38 @@
         <v>14</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="5">
-        <f>COUNTIF(Raw!$S$6:$S$15,Question!F$1)</f>
-        <v>3</v>
-      </c>
-      <c r="G17" s="8">
-        <f>COUNTIF(Raw!$S$6:$S$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="F17" s="9">
+        <v>0.26473757999999997</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="5">
         <f>COUNTIF(Raw!$S$6:$S$15,Question!H$1)</f>
-        <v>5</v>
-      </c>
-      <c r="I17" s="8">
+        <v>3</v>
+      </c>
+      <c r="I17" s="6">
         <f>COUNTIF(Raw!$S$6:$S$15,Question!I$1)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="4">
         <f>COUNTIF(Raw!$S$6:$S$15,Question!J$1)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
+        <v>5</v>
+      </c>
+      <c r="K17" s="6">
         <f>COUNTIF(Raw!$S$6:$S$15,Question!K$1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
+        <f>COUNTIF(Raw!$S$6:$S$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <f>COUNTIF(Raw!$S$6:$S$15,Question!M$1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2527,32 +2641,38 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="4">
-        <f>COUNTIF(Raw!$T$6:$T$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G18" s="8">
-        <f>COUNTIF(Raw!$T$6:$T$15,Question!G$1)</f>
+      <c r="F18" s="9">
+        <v>0.32567259999999998</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="4">
+        <f>COUNTIF(Raw!$T$6:$T$15,Question!H$1)</f>
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <f>COUNTIF(Raw!$T$6:$T$15,Question!I$1)</f>
         <v>1</v>
       </c>
-      <c r="H18" s="8">
-        <f>COUNTIF(Raw!$T$6:$T$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="8">
-        <f>COUNTIF(Raw!$T$6:$T$15,Question!I$1)</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="J18" s="6">
         <f>COUNTIF(Raw!$T$6:$T$15,Question!J$1)</f>
-        <v>4</v>
-      </c>
-      <c r="K18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
         <f>COUNTIF(Raw!$T$6:$T$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18" s="4">
+        <f>COUNTIF(Raw!$T$6:$T$15,Question!L$1)</f>
+        <v>4</v>
+      </c>
+      <c r="M18" s="6">
+        <f>COUNTIF(Raw!$T$6:$T$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2562,32 +2682,38 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="4">
-        <f>COUNTIF(Raw!$U$6:$U$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G19" s="8">
-        <f>COUNTIF(Raw!$U$6:$U$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="8">
+      <c r="F19" s="9">
+        <v>0.3138666</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="4">
         <f>COUNTIF(Raw!$U$6:$U$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
+        <v>5</v>
+      </c>
+      <c r="I19" s="6">
         <f>COUNTIF(Raw!$U$6:$U$15,Question!I$1)</f>
-        <v>5</v>
-      </c>
-      <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="J19" s="6">
         <f>COUNTIF(Raw!$U$6:$U$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="4">
         <f>COUNTIF(Raw!$U$6:$U$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L19" s="6">
+        <f>COUNTIF(Raw!$U$6:$U$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="6">
+        <f>COUNTIF(Raw!$U$6:$U$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2601,32 +2727,38 @@
         <v>4</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="4">
-        <f>COUNTIF(Raw!$V$6:$V$15,Question!F$1)</f>
-        <v>3</v>
-      </c>
-      <c r="G20" s="8">
-        <f>COUNTIF(Raw!$V$6:$V$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="8">
+      <c r="F20" s="9">
+        <v>0.32446461999999998</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="4">
         <f>COUNTIF(Raw!$V$6:$V$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="8">
+        <v>3</v>
+      </c>
+      <c r="I20" s="6">
         <f>COUNTIF(Raw!$V$6:$V$15,Question!I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
+        <f>COUNTIF(Raw!$V$6:$V$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <f>COUNTIF(Raw!$V$6:$V$15,Question!K$1)</f>
         <v>1</v>
       </c>
-      <c r="J20" s="4">
-        <f>COUNTIF(Raw!$V$6:$V$15,Question!J$1)</f>
-        <v>2</v>
-      </c>
-      <c r="K20" s="8">
-        <f>COUNTIF(Raw!$V$6:$V$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20" s="4">
+        <f>COUNTIF(Raw!$V$6:$V$15,Question!L$1)</f>
+        <v>2</v>
+      </c>
+      <c r="M20" s="6">
+        <f>COUNTIF(Raw!$V$6:$V$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2638,13 +2770,11 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="4">
-        <f>COUNTIF(Raw!$W$6:$W$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <f>COUNTIF(Raw!$W$6:$W$15,Question!G$1)</f>
-        <v>0</v>
+      <c r="F21" s="9">
+        <v>0.32988998000000003</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="H21" s="4">
         <f>COUNTIF(Raw!$W$6:$W$15,Question!H$1)</f>
@@ -2662,8 +2792,16 @@
         <f>COUNTIF(Raw!$W$6:$W$15,Question!K$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" s="4">
+        <f>COUNTIF(Raw!$W$6:$W$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <f>COUNTIF(Raw!$W$6:$W$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2675,32 +2813,38 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="8">
-        <f>COUNTIF(Raw!$X$6:$X$15,Question!F$1)</f>
+      <c r="F22" s="9">
+        <v>0.32454988000000001</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="6">
+        <f>COUNTIF(Raw!$X$6:$X$15,Question!H$1)</f>
         <v>1</v>
-      </c>
-      <c r="G22" s="4">
-        <f>COUNTIF(Raw!$X$6:$X$15,Question!G$1)</f>
-        <v>2</v>
-      </c>
-      <c r="H22" s="8">
-        <f>COUNTIF(Raw!$X$6:$X$15,Question!H$1)</f>
-        <v>0</v>
       </c>
       <c r="I22" s="4">
         <f>COUNTIF(Raw!$X$6:$X$15,Question!I$1)</f>
-        <v>3</v>
-      </c>
-      <c r="J22" s="8">
+        <v>2</v>
+      </c>
+      <c r="J22" s="6">
         <f>COUNTIF(Raw!$X$6:$X$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="4">
         <f>COUNTIF(Raw!$X$6:$X$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="L22" s="6">
+        <f>COUNTIF(Raw!$X$6:$X$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <f>COUNTIF(Raw!$X$6:$X$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2712,15 +2856,13 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="8">
-        <f>COUNTIF(Raw!$Y$6:$Y$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <f>COUNTIF(Raw!$Y$6:$Y$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H23" s="8">
+      <c r="F23" s="9">
+        <v>0.35506927999999999</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="6">
         <f>COUNTIF(Raw!$Y$6:$Y$15,Question!H$1)</f>
         <v>0</v>
       </c>
@@ -2728,16 +2870,24 @@
         <f>COUNTIF(Raw!$Y$6:$Y$15,Question!I$1)</f>
         <v>5</v>
       </c>
-      <c r="J23" s="8">
+      <c r="J23" s="6">
         <f>COUNTIF(Raw!$Y$6:$Y$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="4">
         <f>COUNTIF(Raw!$Y$6:$Y$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L23" s="6">
+        <f>COUNTIF(Raw!$Y$6:$Y$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="6">
+        <f>COUNTIF(Raw!$Y$6:$Y$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2749,32 +2899,38 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="4">
-        <f>COUNTIF(Raw!$Z$6:$Z$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G24" s="8">
-        <f>COUNTIF(Raw!$Z$6:$Z$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="8">
+      <c r="F24" s="9">
+        <v>0.32054572999999997</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="4">
         <f>COUNTIF(Raw!$Z$6:$Z$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
+        <v>5</v>
+      </c>
+      <c r="I24" s="6">
         <f>COUNTIF(Raw!$Z$6:$Z$15,Question!I$1)</f>
-        <v>2</v>
-      </c>
-      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
         <f>COUNTIF(Raw!$Z$6:$Z$15,Question!J$1)</f>
-        <v>3</v>
-      </c>
-      <c r="K24" s="8">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
         <f>COUNTIF(Raw!$Z$6:$Z$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="L24" s="5">
+        <f>COUNTIF(Raw!$Z$6:$Z$15,Question!L$1)</f>
+        <v>3</v>
+      </c>
+      <c r="M24" s="6">
+        <f>COUNTIF(Raw!$Z$6:$Z$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2786,32 +2942,38 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="8">
-        <f>COUNTIF(Raw!$AA$6:$AA$15,Question!F$1)</f>
-        <v>2</v>
-      </c>
-      <c r="G25" s="4">
-        <f>COUNTIF(Raw!$AA$6:$AA$15,Question!G$1)</f>
-        <v>4</v>
-      </c>
-      <c r="H25" s="8">
+      <c r="F25" s="9">
+        <v>0.29783700000000002</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="6">
         <f>COUNTIF(Raw!$AA$6:$AA$15,Question!H$1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" s="4">
         <f>COUNTIF(Raw!$AA$6:$AA$15,Question!I$1)</f>
         <v>4</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="6">
         <f>COUNTIF(Raw!$AA$6:$AA$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="4">
         <f>COUNTIF(Raw!$AA$6:$AA$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="L25" s="6">
+        <f>COUNTIF(Raw!$AA$6:$AA$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="6">
+        <f>COUNTIF(Raw!$AA$6:$AA$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2823,32 +2985,38 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="4">
-        <f>COUNTIF(Raw!$AB$6:$AB$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G26" s="8">
-        <f>COUNTIF(Raw!$AB$6:$AB$15,Question!G$1)</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="8">
+      <c r="F26" s="9">
+        <v>0.33302969999999998</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="4">
         <f>COUNTIF(Raw!$AB$6:$AB$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="8">
+        <v>5</v>
+      </c>
+      <c r="I26" s="6">
         <f>COUNTIF(Raw!$AB$6:$AB$15,Question!I$1)</f>
         <v>1</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="6">
         <f>COUNTIF(Raw!$AB$6:$AB$15,Question!J$1)</f>
-        <v>3</v>
-      </c>
-      <c r="K26" s="8">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
         <f>COUNTIF(Raw!$AB$6:$AB$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="L26" s="4">
+        <f>COUNTIF(Raw!$AB$6:$AB$15,Question!L$1)</f>
+        <v>3</v>
+      </c>
+      <c r="M26" s="6">
+        <f>COUNTIF(Raw!$AB$6:$AB$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2860,32 +3028,38 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="8">
-        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!F$1)</f>
+      <c r="F27" s="9">
+        <v>0.32405338</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="6">
+        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!H$1)</f>
         <v>1</v>
-      </c>
-      <c r="G27" s="4">
-        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!G$1)</f>
-        <v>4</v>
-      </c>
-      <c r="H27" s="8">
-        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!H$1)</f>
-        <v>0</v>
       </c>
       <c r="I27" s="4">
         <f>COUNTIF(Raw!$AC$6:$AC$15,Question!I$1)</f>
         <v>4</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="6">
         <f>COUNTIF(Raw!$AC$6:$AC$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!K$1)</f>
+        <v>4</v>
+      </c>
+      <c r="L27" s="6">
+        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K27" s="8">
-        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M27" s="6">
+        <f>COUNTIF(Raw!$AC$6:$AC$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2897,32 +3071,38 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="4">
-        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!F$1)</f>
-        <v>5</v>
-      </c>
-      <c r="G28" s="8">
-        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="8">
+      <c r="F28" s="9">
+        <v>0.33782964999999998</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="4">
         <f>COUNTIF(Raw!$AD$6:$AD$15,Question!H$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
+        <v>5</v>
+      </c>
+      <c r="I28" s="6">
         <f>COUNTIF(Raw!$AD$6:$AD$15,Question!I$1)</f>
-        <v>4</v>
-      </c>
-      <c r="J28" s="8">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6">
         <f>COUNTIF(Raw!$AD$6:$AD$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!K$1)</f>
+        <v>4</v>
+      </c>
+      <c r="L28" s="6">
+        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K28" s="8">
-        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M28" s="6">
+        <f>COUNTIF(Raw!$AD$6:$AD$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2932,32 +3112,38 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="8">
-        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="8">
-        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!G$1)</f>
+      <c r="F29" s="9">
+        <v>0.29702643000000001</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="6">
+        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="6">
+        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!I$1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="4">
-        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!H$1)</f>
-        <v>5</v>
-      </c>
-      <c r="I29" s="8">
-        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!I$1)</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="8">
+      <c r="J29" s="4">
         <f>COUNTIF(Raw!$AE$6:$AE$15,Question!J$1)</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
+        <v>5</v>
+      </c>
+      <c r="K29" s="6">
         <f>COUNTIF(Raw!$AE$6:$AE$15,Question!K$1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6">
+        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
+        <f>COUNTIF(Raw!$AE$6:$AE$15,Question!M$1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2967,32 +3153,38 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="8">
-        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!F$1)</f>
+      <c r="F30" s="9">
+        <v>0.33168690000000001</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="6">
+        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!H$1)</f>
         <v>1</v>
-      </c>
-      <c r="G30" s="4">
-        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!G$1)</f>
-        <v>4</v>
-      </c>
-      <c r="H30" s="8">
-        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!H$1)</f>
-        <v>0</v>
       </c>
       <c r="I30" s="4">
         <f>COUNTIF(Raw!$AF$6:$AF$15,Question!I$1)</f>
         <v>4</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="6">
         <f>COUNTIF(Raw!$AF$6:$AF$15,Question!J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!K$1)</f>
+        <v>4</v>
+      </c>
+      <c r="L30" s="6">
+        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!L$1)</f>
         <v>1</v>
       </c>
-      <c r="K30" s="8">
-        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!K$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M30" s="6">
+        <f>COUNTIF(Raw!$AF$6:$AF$15,Question!M$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3004,15 +3196,13 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="8">
-        <f>COUNTIF(Raw!$AG$6:$AG$15,Question!F$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="4">
-        <f>COUNTIF(Raw!$AG$6:$AG$15,Question!G$1)</f>
-        <v>5</v>
-      </c>
-      <c r="H31" s="8">
+      <c r="F31" s="9">
+        <v>0.35066795000000001</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="6">
         <f>COUNTIF(Raw!$AG$6:$AG$15,Question!H$1)</f>
         <v>0</v>
       </c>
@@ -3020,17 +3210,25 @@
         <f>COUNTIF(Raw!$AG$6:$AG$15,Question!I$1)</f>
         <v>5</v>
       </c>
-      <c r="J31" s="8">
+      <c r="J31" s="6">
         <f>COUNTIF(Raw!$AG$6:$AG$15,Question!J$1)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="4">
         <f>COUNTIF(Raw!$AG$6:$AG$15,Question!K$1)</f>
+        <v>5</v>
+      </c>
+      <c r="L31" s="6">
+        <f>COUNTIF(Raw!$AG$6:$AG$15,Question!L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="6">
+        <f>COUNTIF(Raw!$AG$6:$AG$15,Question!M$1)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
+  <sortState ref="A2:K31">
     <sortCondition ref="A1:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>